<commit_message>
[New] Product configurator page and updated product manager
</commit_message>
<xml_diff>
--- a/Planificación Rasher.xlsx
+++ b/Planificación Rasher.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIGUEL\Desktop\Kyrema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B123BF6A-8C67-45E9-ADD9-7A3D5719BFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC0C691-E556-4C07-A30C-BEF7162D33B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1714033532260_BindMessage" sheetId="1" r:id="rId1"/>
@@ -145,12 +145,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -238,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -252,6 +258,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -692,14 +701,14 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="10">
+      <c r="C7" s="12"/>
+      <c r="D7" s="13">
         <v>45439</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="13">
         <v>45440</v>
       </c>
     </row>
@@ -721,14 +730,14 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="10">
+      <c r="C11" s="12"/>
+      <c r="D11" s="13">
         <v>45441</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="13">
         <v>45442</v>
       </c>
     </row>

</xml_diff>